<commit_message>
Rewrite of complete code. Add N Current Diagramm
</commit_message>
<xml_diff>
--- a/Excel/Leistungsbedarf.xlsx
+++ b/Excel/Leistungsbedarf.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Leistungsbedarf" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Spannungsfall" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Leitungsberechnung" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="N-Leiterstrom" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t xml:space="preserve">Leistungsbedarf UV-1 Coffee-Lounge</t>
   </si>
@@ -109,13 +110,49 @@
   </si>
   <si>
     <t xml:space="preserve">Gesamtstrom mit Reserve:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cos φ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winkel φ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wirkstrom Iw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blindströme Ibl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scheinstrom I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X Schein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y Schein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I L1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kapazitiv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I L2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I L3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="13">
+  <numFmts count="12">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="0&quot; Stk.&quot;"/>
@@ -127,10 +164,9 @@
     <numFmt numFmtId="172" formatCode="0&quot; A&quot;"/>
     <numFmt numFmtId="173" formatCode="0.0&quot; mm²&quot;"/>
     <numFmt numFmtId="174" formatCode="0\ %"/>
-    <numFmt numFmtId="175" formatCode="0.00&quot; A&quot;"/>
-    <numFmt numFmtId="176" formatCode="0&quot; mm²&quot;"/>
+    <numFmt numFmtId="175" formatCode="0&quot; mm²&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -156,14 +192,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Consolas"/>
+      <name val="Courier New"/>
       <family val="3"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
-      <name val="Consolas"/>
+      <name val="Courier New"/>
       <family val="3"/>
       <charset val="1"/>
     </font>
@@ -171,7 +207,15 @@
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Consolas"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
       <family val="3"/>
       <charset val="1"/>
     </font>
@@ -314,7 +358,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -411,11 +455,11 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="175" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="175" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="171" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -423,19 +467,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="175" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="175" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="175" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="175" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -447,8 +491,24 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="175" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -549,13 +609,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M1048576"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.91015625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25"/>
@@ -588,7 +648,7 @@
       <c r="L1" s="2"/>
       <c r="M1" s="3" t="n">
         <f aca="true">TODAY()</f>
-        <v>44500</v>
+        <v>44504</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -621,7 +681,7 @@
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
     </row>
-    <row r="4" s="9" customFormat="true" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="9" customFormat="true" ht="26.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -662,7 +722,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="n">
         <v>1</v>
       </c>
@@ -703,7 +763,7 @@
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
     </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="n">
         <v>2</v>
       </c>
@@ -1203,7 +1263,7 @@
       <c r="I22" s="20"/>
       <c r="J22" s="20"/>
     </row>
-    <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="21" t="s">
         <v>17</v>
       </c>
@@ -1229,7 +1289,7 @@
       </c>
       <c r="J23" s="20"/>
     </row>
-    <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="21" t="s">
         <v>19</v>
       </c>
@@ -1253,7 +1313,7 @@
       </c>
       <c r="J24" s="20"/>
     </row>
-    <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="21" t="s">
         <v>21</v>
       </c>
@@ -1274,7 +1334,7 @@
       <c r="I25" s="30"/>
       <c r="J25" s="20"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="21" t="s">
         <v>23</v>
       </c>
@@ -1295,7 +1355,7 @@
       <c r="I26" s="30"/>
       <c r="J26" s="20"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="20"/>
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
@@ -1312,7 +1372,7 @@
       <c r="I27" s="33"/>
       <c r="J27" s="20"/>
     </row>
-    <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="20"/>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
@@ -1324,7 +1384,7 @@
       <c r="I28" s="20"/>
       <c r="J28" s="20"/>
     </row>
-    <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="20"/>
       <c r="B29" s="20"/>
       <c r="C29" s="20"/>
@@ -1336,8 +1396,6 @@
       <c r="I29" s="20"/>
       <c r="J29" s="20"/>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="A1:L2"/>
@@ -1374,14 +1432,14 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="34" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1403,11 +1461,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1417,4 +1475,174 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:O7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="9.26"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="1" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="36" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="K2" s="1" t="e">
+        <f aca="false">IF(NOT(ISBLANK(B2)),DEGREES(ACOS(B2)),)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <f aca="false">IF(NOT(ISBLANK(C2)),DEGREES(ACOS(C2)),)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="37"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="37"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C7:I7"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G13" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2 B4 B6" type="list">
+      <formula1>"Induktiv,Kapazitiv,Ohmisch"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>